<commit_message>
Novos ajustes de exibicao
</commit_message>
<xml_diff>
--- a/files/system/import-clients-sample.xlsx
+++ b/files/system/import-clients-sample.xlsx
@@ -1,24 +1,50 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27921"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{72D7ECE2-5712-4124-875C-7AF74EB957E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
   <si>
     <t>Company name</t>
   </si>
   <si>
+    <t>Contact first name</t>
+  </si>
+  <si>
+    <t>Contact last name</t>
+  </si>
+  <si>
+    <t>Contact email</t>
+  </si>
+  <si>
     <t>Address</t>
   </si>
   <si>
@@ -52,9 +78,21 @@
     <t>Currency Symbol</t>
   </si>
   <si>
+    <t>CNPJ</t>
+  </si>
+  <si>
     <t>Ashton Cox</t>
   </si>
   <si>
+    <t>Ashton</t>
+  </si>
+  <si>
+    <t>Cox</t>
+  </si>
+  <si>
+    <t>client1@demo.com</t>
+  </si>
+  <si>
     <t>Forrest Ray</t>
   </si>
   <si>
@@ -79,6 +117,15 @@
     <t>Bradley Greer</t>
   </si>
   <si>
+    <t>Bradley</t>
+  </si>
+  <si>
+    <t>Greer</t>
+  </si>
+  <si>
+    <t>client2@demo.com</t>
+  </si>
+  <si>
     <t>Aaron Hawkins</t>
   </si>
   <si>
@@ -103,83 +150,56 @@
     <t>Brielle Williamson</t>
   </si>
   <si>
+    <t>Brielle</t>
+  </si>
+  <si>
+    <t>Williamson</t>
+  </si>
+  <si>
+    <t>client3@demo.com</t>
+  </si>
+  <si>
     <t>Bruno Nash</t>
   </si>
   <si>
+    <t>Bruno</t>
+  </si>
+  <si>
+    <t>Nash</t>
+  </si>
+  <si>
+    <t>client4@demo.com</t>
+  </si>
+  <si>
     <t>Cara Stevens</t>
   </si>
   <si>
+    <t>Cara</t>
+  </si>
+  <si>
+    <t>Stevens</t>
+  </si>
+  <si>
+    <t>client5@demo.com</t>
+  </si>
+  <si>
     <t>Cedric Kelly</t>
   </si>
   <si>
-    <t>Contact first name</t>
-  </si>
-  <si>
-    <t>Contact last name</t>
-  </si>
-  <si>
-    <t>Contact email</t>
-  </si>
-  <si>
-    <t>Ashton</t>
-  </si>
-  <si>
-    <t>Cox</t>
-  </si>
-  <si>
-    <t>client1@demo.com</t>
-  </si>
-  <si>
-    <t>client2@demo.com</t>
-  </si>
-  <si>
-    <t>client3@demo.com</t>
-  </si>
-  <si>
-    <t>client4@demo.com</t>
-  </si>
-  <si>
-    <t>client5@demo.com</t>
+    <t>Cedric</t>
+  </si>
+  <si>
+    <t>Kelly</t>
   </si>
   <si>
     <t>client6@demo.com</t>
-  </si>
-  <si>
-    <t>Bradley</t>
-  </si>
-  <si>
-    <t>Greer</t>
-  </si>
-  <si>
-    <t>Brielle</t>
-  </si>
-  <si>
-    <t>Williamson</t>
-  </si>
-  <si>
-    <t>Bruno</t>
-  </si>
-  <si>
-    <t>Nash</t>
-  </si>
-  <si>
-    <t>Cara</t>
-  </si>
-  <si>
-    <t>Stevens</t>
-  </si>
-  <si>
-    <t>Cedric</t>
-  </si>
-  <si>
-    <t>Kelly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,9 +283,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -303,9 +323,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -340,7 +360,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -375,7 +395,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -548,14 +568,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="3" width="19.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" style="1" customWidth="1"/>
@@ -573,291 +593,294 @@
     <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="2" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H2" s="5">
         <v>1234</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="J2" s="5">
         <v>123456789</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="L2" s="5">
         <v>8219</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="H3" s="5">
         <v>1234</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="J3" s="5">
         <v>123456789</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="L3" s="5">
         <v>8219</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="4" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H4" s="5">
         <v>1234</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="J4" s="5">
         <v>123456789</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="L4" s="5">
         <v>8219</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5" s="4" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="H5" s="5">
         <v>1234</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="J5" s="5">
         <v>123456789</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="L5" s="5">
         <v>8219</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="O5" s="5" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6" s="4" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" t="s">
-        <v>41</v>
-      </c>
       <c r="E6" s="5" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H6" s="5">
         <v>1234</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="J6" s="5">
         <v>123456789</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="L6" s="5">
         <v>8219</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="A7" s="4" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>51</v>
@@ -866,40 +889,40 @@
         <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="H7" s="5">
         <v>1234</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="J7" s="5">
         <v>123456789</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="L7" s="5">
         <v>8219</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>